<commit_message>
Plantilla  Azul OK + Transfermarkt
</commit_message>
<xml_diff>
--- a/datos_scouting.xlsx
+++ b/datos_scouting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">García</t>
   </si>
   <si>
-    <t xml:space="preserve">Central Defense</t>
+    <t xml:space="preserve">Central Back</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.transfermarkt.co/simon-garcia/profil/spieler/1202035</t>
@@ -250,7 +250,7 @@
     <t xml:space="preserve">https://www.instagram.com/simongarciav_/</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ssl.gstatic.com/onebox/media/sports/logos/i6-Yda76iPfeYEg4JcNbuw_64x64.png</t>
+    <t xml:space="preserve">images/atleticonacional.png</t>
   </si>
   <si>
     <t xml:space="preserve">images/simongarcia.jpg</t>
@@ -299,6 +299,175 @@
   </si>
   <si>
     <t xml:space="preserve">2022/23|At. Nacional|30|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.transfermarkt.com/juan-lopez/profil/spieler/572814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.instagram.com/p/DIk3lt6OhYi/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/germanbush.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/juanlopez.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">German Busch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€500K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fubstar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Strong 1v1 defending </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">| H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">igh defensive awareness </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">onsistently winning duels </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> stopping attacks and leading the back line. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2024/25|  Germán Busch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">|28|15</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/24|Caldense|30|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/23|Aimoré|30|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esteban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right/left winger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.transfermarkt.us/esteban-mercado/profil/spieler/1007701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.instagram.com/esteban_mercado7/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/junior.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/estebanmercado.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=cCx4VAOW1u4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excellent technique | Strong 1v1 dribbling | High attacking ability | Consistently creating goals and assists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/25|Junior FC|2|15</t>
   </si>
 </sst>
 </file>
@@ -308,7 +477,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +513,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -399,16 +581,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,405 +803,591 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="70.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="48.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="70.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="48.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X2" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y2" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AA2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AC2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AE2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AF2" s="0" t="s">
+      <c r="AF2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>1.86</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="S4" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="T4" s="0" t="n">
+      <c r="T4" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="W4" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="X4" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Z4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="AA4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AB4" s="0" t="s">
+      <c r="AB4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC4" s="0" t="s">
+      <c r="AC4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AD4" s="0" t="s">
+      <c r="AD4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AE4" s="0" t="s">
+      <c r="AE4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AF4" s="0" t="s">
+      <c r="AF4" s="4" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="https://www.transfermarkt.co/simon-garcia/profil/spieler/1202035"/>
     <hyperlink ref="E4" r:id="rId2" display="https://www.instagram.com/simongarciav_/"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://ssl.gstatic.com/onebox/media/sports/logos/i6-Yda76iPfeYEg4JcNbuw_64x64.png"/>
-    <hyperlink ref="R4" r:id="rId4" display="https://www.youtube.com/watch?v=Ed7fPg1LE5o"/>
+    <hyperlink ref="R4" r:id="rId3" display="https://www.youtube.com/watch?v=Ed7fPg1LE5o"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://www.transfermarkt.com/juan-lopez/profil/spieler/572814"/>
+    <hyperlink ref="R5" r:id="rId5" display="https://www.youtube.com/watch?v=Ed7fPg1LE5o"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Plantilla  Azul OK + Juan Lopez + Esteban Mercado
</commit_message>
<xml_diff>
--- a/datos_scouting.xlsx
+++ b/datos_scouting.xlsx
@@ -286,7 +286,7 @@
     <t xml:space="preserve">78.6</t>
   </si>
   <si>
-    <t xml:space="preserve">Solid defensive presence|Leadership and reading of the game|Strong in the air</t>
+    <t xml:space="preserve">Solid defensive presence | Leadership and reading of the game | Strong in the air</t>
   </si>
   <si>
     <t xml:space="preserve">€2M| €3-5M |€10-25M+</t>
@@ -364,7 +364,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">|C</t>
+      <t xml:space="preserve">| C</t>
     </r>
     <r>
       <rPr>
@@ -393,7 +393,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> stopping attacks and leading the back line. </t>
+      <t xml:space="preserve"> Stopping attacks and leading the back line. </t>
     </r>
   </si>
   <si>
@@ -805,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB5" activeCellId="0" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Agregar python generar.py verde
</commit_message>
<xml_diff>
--- a/datos_scouting.xlsx
+++ b/datos_scouting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="122">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -271,130 +271,67 @@
     <t xml:space="preserve">31/12/2026</t>
   </si>
   <si>
+    <t xml:space="preserve">€2.5M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizzor image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=Ed7fPg1LE5o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solid defensive presence | Leadership and reading of the game | Strong in the air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2M| €3-5M |€10-25M+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024/25|At. Nacional|28|15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/23|Sel. Colombia U20|30|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/23|At. Nacional|30|10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.transfermarkt.com/juan-lopez/profil/spieler/572814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.instagram.com/p/DIk3lt6OhYi/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/germanbush.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/juanlopez.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">German Busch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€500K</t>
+  </si>
+  <si>
     <t xml:space="preserve">€2M</t>
   </si>
   <si>
-    <t xml:space="preserve">Vizzor image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=Ed7fPg1LE5o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solid defensive presence | Leadership and reading of the game | Strong in the air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€2M| €3-5M |€10-25M+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024/25|At. Nacional|28|15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022/23|Sel. Colombia U20|30|10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022/23|At. Nacional|30|10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lopez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.transfermarkt.com/juan-lopez/profil/spieler/572814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.instagram.com/p/DIk3lt6OhYi/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">images/germanbush.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">images/juanlopez.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">German Busch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€500K</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fubstar</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Strong 1v1 defending </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">| H</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">igh defensive awareness </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">| C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">onsistently winning duels </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">|</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Stopping attacks and leading the back line. </t>
-    </r>
+    <t xml:space="preserve">Strong 1v1 defending | High defensive awareness | Consistently winning duels | Stopping attacks and leading the back line. </t>
   </si>
   <si>
     <r>
@@ -477,7 +414,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,12 +451,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -606,7 +537,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -805,8 +736,8 @@
   </sheetPr>
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB5" activeCellId="0" sqref="AB5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1241,10 +1172,10 @@
         <v>82</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>85</v>
@@ -1277,42 +1208,42 @@
         <v>87</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AC5" s="1" t="s">
         <v>89</v>
       </c>
       <c r="AD5" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>78</v>
@@ -1327,22 +1258,22 @@
         <v>79</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>100</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S6" s="1" t="n">
         <v>75</v>
@@ -1366,19 +1297,19 @@
         <v>85</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC6" s="1" t="s">
         <v>89</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>